<commit_message>
fix: calculator for multiple sheets
</commit_message>
<xml_diff>
--- a/packages/calculator/src/marks.xlsx
+++ b/packages/calculator/src/marks.xlsx
@@ -5,13 +5,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="A" sheetId="1" r:id="rId4"/>
+    <sheet name="B" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
   <si>
     <r>
       <rPr>
@@ -754,6 +755,231 @@
       </rPr>
       <t>Pol</t>
     </r>
+  </si>
+  <si>
+    <t>Listen carefully to the Froggy’s halloween story and can explain the sequence.</t>
+  </si>
+  <si>
+    <t>Calvo</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>Lluna</t>
+  </si>
+  <si>
+    <t>de la Cruz</t>
+  </si>
+  <si>
+    <t>Borjas</t>
+  </si>
+  <si>
+    <t>Laia</t>
+  </si>
+  <si>
+    <t>Fortunato</t>
+  </si>
+  <si>
+    <t>Yeste</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Frigola</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Canovas</t>
+  </si>
+  <si>
+    <t>Arian</t>
+  </si>
+  <si>
+    <t>Guerra</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Isern</t>
+  </si>
+  <si>
+    <t>Abelló</t>
+  </si>
+  <si>
+    <t>Martí</t>
+  </si>
+  <si>
+    <t>Jimenez</t>
+  </si>
+  <si>
+    <t>Lorente</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Llupià</t>
+  </si>
+  <si>
+    <t>Subirats</t>
+  </si>
+  <si>
+    <t>Lluc</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Cabrera</t>
+  </si>
+  <si>
+    <t>Aritz</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>Cañisá</t>
+  </si>
+  <si>
+    <t>Júlia</t>
+  </si>
+  <si>
+    <t>Majait</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Martín</t>
+  </si>
+  <si>
+    <t>Gol</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Gerard</t>
+  </si>
+  <si>
+    <t>Mestres</t>
+  </si>
+  <si>
+    <t>Parra</t>
+  </si>
+  <si>
+    <t>Aina</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Sancho</t>
+  </si>
+  <si>
+    <t>Olaf</t>
+  </si>
+  <si>
+    <t>Nafid</t>
+  </si>
+  <si>
+    <t>Mouslem</t>
+  </si>
+  <si>
+    <t>Ortega</t>
+  </si>
+  <si>
+    <t>Carrillo</t>
+  </si>
+  <si>
+    <t>Ainara</t>
+  </si>
+  <si>
+    <t>Ortiz</t>
+  </si>
+  <si>
+    <t>Portabales</t>
+  </si>
+  <si>
+    <t>Alexandra</t>
+  </si>
+  <si>
+    <t>Larruy</t>
+  </si>
+  <si>
+    <t>Joana</t>
+  </si>
+  <si>
+    <t>Passerini</t>
+  </si>
+  <si>
+    <t>Millon</t>
+  </si>
+  <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>Rioja</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Roig</t>
+  </si>
+  <si>
+    <t>Castaño</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>Sánchez</t>
+  </si>
+  <si>
+    <t>Oviedo</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Amador</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Tataru</t>
+  </si>
+  <si>
+    <t>Arina</t>
+  </si>
+  <si>
+    <t>Zapater</t>
+  </si>
+  <si>
+    <t>González</t>
+  </si>
+  <si>
+    <t>Bruna</t>
   </si>
 </sst>
 </file>
@@ -763,7 +989,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -785,8 +1011,13 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,8 +1036,32 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -844,13 +1099,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -878,6 +1170,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,6 +1223,10 @@
       <rgbColor rgb="fff1f1f1"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="fff79646"/>
+      <rgbColor rgb="ff9bbb59"/>
+      <rgbColor rgb="ff4f81bd"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -3548,4 +3877,1790 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:U28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="21" width="16.3516" style="9" customWidth="1"/>
+    <col min="22" max="16384" width="16.3516" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="62.7" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="10">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="10">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="10">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="11">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="12">
+        <v>88</v>
+      </c>
+      <c r="L1" t="s" s="13">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s" s="13">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s" s="13">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s" s="13">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="Q1" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s" s="13">
+        <v>15</v>
+      </c>
+      <c r="S1" t="s" s="13">
+        <v>16</v>
+      </c>
+      <c r="T1" t="s" s="13">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="21" customHeight="1">
+      <c r="A2" t="s" s="16">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s" s="17">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s" s="17">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S2" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U2" s="7"/>
+    </row>
+    <row r="3" ht="21" customHeight="1">
+      <c r="A3" t="s" s="16">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s" s="17">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s" s="17">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T3" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U3" s="18"/>
+    </row>
+    <row r="4" ht="21" customHeight="1">
+      <c r="A4" t="s" s="16">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s" s="17">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s" s="17">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="P4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="R4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S4" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="T4" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" ht="21" customHeight="1">
+      <c r="A5" t="s" s="16">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s" s="17">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s" s="17">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="S5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T5" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" ht="21" customHeight="1">
+      <c r="A6" t="s" s="16">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s" s="17">
+        <v>102</v>
+      </c>
+      <c r="C6" t="s" s="17">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T6" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U6" s="7"/>
+    </row>
+    <row r="7" ht="21" customHeight="1">
+      <c r="A7" t="s" s="16">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s" s="17">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s" s="17">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="S7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T7" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="U7" s="7"/>
+    </row>
+    <row r="8" ht="21" customHeight="1">
+      <c r="A8" t="s" s="16">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s" s="17">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s" s="17">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="S8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" ht="21" customHeight="1">
+      <c r="A9" t="s" s="16">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s" s="17">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s" s="17">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="N9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O9" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S9" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T9" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" ht="21" customHeight="1">
+      <c r="A10" t="s" s="16">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s" s="17">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s" s="17">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="P10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S10" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T10" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" ht="21" customHeight="1">
+      <c r="A11" t="s" s="16">
+        <v>115</v>
+      </c>
+      <c r="B11" t="s" s="17">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s" s="17">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="N11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q11" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R11" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S11" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T11" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" ht="21" customHeight="1">
+      <c r="A12" t="s" s="16">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s" s="17">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s" s="17">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M12" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O12" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R12" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S12" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T12" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" ht="21" customHeight="1">
+      <c r="A13" t="s" s="16">
+        <v>121</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" t="s" s="17">
+        <v>122</v>
+      </c>
+      <c r="D13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="N13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="P13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="R13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S13" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="T13" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" ht="21" customHeight="1">
+      <c r="A14" t="s" s="16">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s" s="17">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s" s="17">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="N14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O14" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R14" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S14" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T14" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" ht="21" customHeight="1">
+      <c r="A15" t="s" s="16">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s" s="17">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s" s="17">
+        <v>127</v>
+      </c>
+      <c r="D15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="I15" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J15" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="N15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="O15" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="P15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="R15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S15" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T15" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U15" s="7"/>
+    </row>
+    <row r="16" ht="21" customHeight="1">
+      <c r="A16" t="s" s="16">
+        <v>128</v>
+      </c>
+      <c r="B16" t="s" s="17">
+        <v>129</v>
+      </c>
+      <c r="C16" t="s" s="17">
+        <v>130</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="N16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="P16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="S16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T16" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="U16" s="7"/>
+    </row>
+    <row r="17" ht="21" customHeight="1">
+      <c r="A17" t="s" s="16">
+        <v>131</v>
+      </c>
+      <c r="B17" t="s" s="17">
+        <v>132</v>
+      </c>
+      <c r="C17" t="s" s="17">
+        <v>133</v>
+      </c>
+      <c r="D17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J17" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L17" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O17" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="P17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q17" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R17" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S17" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T17" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" ht="21" customHeight="1">
+      <c r="A18" t="s" s="16">
+        <v>134</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" t="s" s="17">
+        <v>135</v>
+      </c>
+      <c r="D18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="I18" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J18" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="N18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="O18" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="P18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="R18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S18" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="T18" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" ht="21" customHeight="1">
+      <c r="A19" t="s" s="16">
+        <v>136</v>
+      </c>
+      <c r="B19" t="s" s="17">
+        <v>137</v>
+      </c>
+      <c r="C19" t="s" s="17">
+        <v>138</v>
+      </c>
+      <c r="D19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J19" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L19" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S19" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T19" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" ht="21" customHeight="1">
+      <c r="A20" t="s" s="16">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s" s="17">
+        <v>140</v>
+      </c>
+      <c r="C20" t="s" s="17">
+        <v>141</v>
+      </c>
+      <c r="D20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="L20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="N20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="O20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="P20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="Q20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="R20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="S20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T20" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="U20" s="7"/>
+    </row>
+    <row r="21" ht="21" customHeight="1">
+      <c r="A21" t="s" s="16">
+        <v>129</v>
+      </c>
+      <c r="B21" t="s" s="17">
+        <v>142</v>
+      </c>
+      <c r="C21" t="s" s="17">
+        <v>143</v>
+      </c>
+      <c r="D21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J21" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L21" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S21" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T21" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U21" s="7"/>
+    </row>
+    <row r="22" ht="21" customHeight="1">
+      <c r="A22" t="s" s="16">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s" s="17">
+        <v>145</v>
+      </c>
+      <c r="C22" t="s" s="17">
+        <v>146</v>
+      </c>
+      <c r="D22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I22" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J22" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L22" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S22" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T22" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" ht="21" customHeight="1">
+      <c r="A23" t="s" s="16">
+        <v>147</v>
+      </c>
+      <c r="B23" t="s" s="17">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s" s="17">
+        <v>148</v>
+      </c>
+      <c r="D23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H23" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I23" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J23" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S23" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T23" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" ht="21" customHeight="1">
+      <c r="A24" t="s" s="16">
+        <v>149</v>
+      </c>
+      <c r="B24" t="s" s="17">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s" s="17">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H24" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I24" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="M24" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="N24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O24" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="P24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q24" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R24" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S24" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T24" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U24" s="7"/>
+    </row>
+    <row r="25" ht="21" customHeight="1">
+      <c r="A25" t="s" s="16">
+        <v>152</v>
+      </c>
+      <c r="B25" t="s" s="17">
+        <v>153</v>
+      </c>
+      <c r="C25" t="s" s="17">
+        <v>154</v>
+      </c>
+      <c r="D25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="I25" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="L25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="M25" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="N25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="O25" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="P25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="R25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S25" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="T25" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U25" s="7"/>
+    </row>
+    <row r="26" ht="21" customHeight="1">
+      <c r="A26" t="s" s="16">
+        <v>155</v>
+      </c>
+      <c r="B26" t="s" s="17">
+        <v>156</v>
+      </c>
+      <c r="C26" t="s" s="17">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="I26" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="L26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="M26" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="N26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="O26" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="P26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="Q26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="R26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="S26" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="T26" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="U26" s="7"/>
+    </row>
+    <row r="27" ht="21" customHeight="1">
+      <c r="A27" t="s" s="16">
+        <v>158</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" t="s" s="17">
+        <v>159</v>
+      </c>
+      <c r="D27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I27" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J27" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S27" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T27" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" ht="21" customHeight="1">
+      <c r="A28" t="s" s="16">
+        <v>160</v>
+      </c>
+      <c r="B28" t="s" s="17">
+        <v>161</v>
+      </c>
+      <c r="C28" t="s" s="17">
+        <v>162</v>
+      </c>
+      <c r="D28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="I28" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="J28" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L28" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="M28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="N28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="O28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="P28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="R28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="S28" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="T28" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="U28" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>